<commit_message>
Update Spreadsheets with 2024/2025 inflation data
</commit_message>
<xml_diff>
--- a/Data/mcquarrie_real_nom_stock_bond_returns_1793_2024.xlsx
+++ b/Data/mcquarrie_real_nom_stock_bond_returns_1793_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherifarkam/Desktop/Data_Science/Projects/Repositories/Stocks_Bonds_Mcquarrie_Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AEBBD1-A378-4640-9FD4-193665E16DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718469F6-EC57-D946-94D1-9890BFBA1EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20180" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks v Bonds Periods" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>From the 'not seasonally adjusted' numbers</t>
+          <t>From the 'not seasonally adjusted' BLS Consumer Price Index for All Urban Consumers numbers</t>
         </r>
       </text>
     </comment>
@@ -484,7 +484,7 @@
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,13 +530,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -712,12 +705,12 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,7 +1116,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1199,115 +1192,115 @@
       </c>
       <c r="C4" s="2">
         <f>RATE(25,,'Real Returns 1792-2025'!J210,-'Real Returns 1792-2025'!J235)</f>
-        <v>5.2099382840357013E-2</v>
+        <v>5.1864136651233031E-2</v>
       </c>
       <c r="D4" s="2">
         <f>RATE(25,,'Real Returns 1792-2025'!K210,-'Real Returns 1792-2025'!K235)</f>
-        <v>3.2898697621294722E-2</v>
+        <v>3.2667744646386471E-2</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="0"/>
-        <v>1.9200685219062291E-2</v>
+        <v>1.919639200484656E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="43">
+      <c r="A5" s="42">
         <v>1793</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="42">
         <v>2025</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="43">
         <f>RATE(232,,'Real Returns 1792-2025'!J3,-'Real Returns 1792-2025'!J235)</f>
-        <v>6.1793401409786126E-2</v>
-      </c>
-      <c r="D5" s="44">
+        <v>6.1767815480094468E-2</v>
+      </c>
+      <c r="D5" s="43">
         <f>RATE(232,,'Real Returns 1792-2025'!K3,-'Real Returns 1792-2025'!K235)</f>
-        <v>3.9535356396241408E-2</v>
-      </c>
-      <c r="E5" s="44">
-        <f t="shared" si="0"/>
-        <v>2.2258045013544718E-2</v>
+        <v>3.951030681644041E-2</v>
+      </c>
+      <c r="E5" s="43">
+        <f t="shared" si="0"/>
+        <v>2.2257508663654058E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="45">
+      <c r="A6" s="44">
         <v>1793</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <v>1942</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="45">
         <f>RATE(149,,'Real Returns 1792-2025'!J3,-'Real Returns 1792-2025'!J152)</f>
         <v>5.3550463589011325E-2</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="45">
         <f>RATE(149,,'Real Returns 1792-2025'!K3,-'Real Returns 1792-2025'!K152)</f>
         <v>5.1916700146403157E-2</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="45">
         <f t="shared" si="0"/>
         <v>1.6337634426081687E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="45">
+      <c r="A7" s="44">
         <v>1942</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <v>2025</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="45">
         <f>RATE(83,,'Real Returns 1792-2025'!J152,-'Real Returns 1792-2025'!J235)</f>
-        <v>7.6753106713136426E-2</v>
-      </c>
-      <c r="D7" s="46">
+        <v>7.6680583370517433E-2</v>
+      </c>
+      <c r="D7" s="45">
         <f>RATE(83,,'Real Returns 1792-2025'!K152,-'Real Returns 1792-2025'!K235)</f>
-        <v>1.7673095768354269E-2</v>
-      </c>
-      <c r="E7" s="46">
-        <f t="shared" si="0"/>
-        <v>5.9080010944782158E-2</v>
+        <v>1.7604551685094335E-2</v>
+      </c>
+      <c r="E7" s="45">
+        <f t="shared" si="0"/>
+        <v>5.9076031685423094E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45">
+      <c r="A8" s="44">
         <v>1942</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>1982</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="46">
         <f>RATE(40,,'Real Returns 1792-2025'!J152,-'Real Returns 1792-2025'!J192)</f>
         <v>6.690855476577387E-2</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="46">
         <f>RATE(40,,'Real Returns 1792-2025'!K152,-'Real Returns 1792-2025'!K192)</f>
         <v>-2.1045299583573766E-2</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="45">
         <f t="shared" si="0"/>
         <v>8.7953854349347632E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="45">
+      <c r="A9" s="44">
         <v>1982</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>2025</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="46">
         <f>RATE(43,,'Real Returns 1792-2025'!J192,-'Real Returns 1792-2025'!J235)</f>
-        <v>8.5992364237042526E-2</v>
-      </c>
-      <c r="D9" s="47">
+        <v>8.5851180562127774E-2</v>
+      </c>
+      <c r="D9" s="46">
         <f>RATE(43,,'Real Returns 1792-2025'!K192,-'Real Returns 1792-2025'!K235)</f>
-        <v>5.5063768248560054E-2</v>
-      </c>
-      <c r="E9" s="46">
-        <f t="shared" si="0"/>
-        <v>3.0928595988482473E-2</v>
+        <v>5.4926605424079983E-2</v>
+      </c>
+      <c r="E9" s="45">
+        <f t="shared" si="0"/>
+        <v>3.0924575138047791E-2</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2300,8 +2293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2406,11 +2399,11 @@
       </c>
       <c r="J3" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$L:$L)</f>
-        <v>6.2788502948706554E-2</v>
+        <v>6.2785760901891377E-2</v>
       </c>
       <c r="K3" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$M:$M)</f>
-        <v>4.2885687031009416E-2</v>
+        <v>4.2883213667721874E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2451,11 +2444,11 @@
       </c>
       <c r="J4" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$N:$N)</f>
-        <v>6.184834435926307E-2</v>
+        <v>6.1847353925529619E-2</v>
       </c>
       <c r="K4" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$O:$O)</f>
-        <v>4.1827939035677851E-2</v>
+        <v>4.1826987906128932E-2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2496,11 +2489,11 @@
       </c>
       <c r="J5" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$P:$P)</f>
-        <v>6.0820620963663925E-2</v>
+        <v>6.081996089239422E-2</v>
       </c>
       <c r="K5" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$Q:$Q)</f>
-        <v>3.9474826394361652E-2</v>
+        <v>3.9474192014525733E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2541,11 +2534,11 @@
       </c>
       <c r="J6" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$R:$R)</f>
-        <v>6.1973719792752374E-2</v>
+        <v>6.1973269856479725E-2</v>
       </c>
       <c r="K6" s="2">
         <f>AVERAGE('Real Returns 1792-2025'!$S:$S)</f>
-        <v>3.9312545011899666E-2</v>
+        <v>3.9312114753779721E-2</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3548,8 +3541,8 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M163" sqref="M163"/>
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K232" sqref="K232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17359,60 +17352,60 @@
         <v>2025</v>
       </c>
       <c r="D235" s="41">
-        <v>315.89999999999998</v>
+        <v>317.67099999999999</v>
       </c>
       <c r="E235">
-        <v>1.0242626054983999</v>
+        <v>1.0300048311215011</v>
       </c>
       <c r="F235">
         <v>0.26160903455164708</v>
       </c>
       <c r="G235">
-        <v>0.23172419629412899</v>
+        <v>0.22485739525897963</v>
       </c>
       <c r="H235">
         <v>-7.0091368427013245E-3</v>
       </c>
       <c r="I235">
-        <v>-3.0530981189032635E-2</v>
+        <v>-3.5935722674135917E-2</v>
       </c>
       <c r="J235">
-        <v>1099727.5825945265</v>
+        <v>1093596.6561052501</v>
       </c>
       <c r="K235">
-        <v>8066.952243452889</v>
+        <v>8021.9793865564288</v>
       </c>
       <c r="L235" s="2">
         <f>RATE(10,,J225,-'Real Returns 1792-2025'!$J235)</f>
-        <v>9.4074062604235661E-2</v>
+        <v>9.3462586164452369E-2</v>
       </c>
       <c r="M235" s="2">
         <f>RATE(10,,K225,-'Real Returns 1792-2025'!$K235)</f>
-        <v>-1.313040851882305E-2</v>
+        <v>-1.3681968531945338E-2</v>
       </c>
       <c r="N235" s="2">
         <f>RATE(30,,J205,-'Real Returns 1792-2025'!$J235)</f>
-        <v>7.9018234173736213E-2</v>
+        <v>7.8817176125844851E-2</v>
       </c>
       <c r="O235" s="2">
         <f>RATE(30,,K205,-'Real Returns 1792-2025'!$K235)</f>
-        <v>3.6198679275229163E-2</v>
+        <v>3.6005599976797545E-2</v>
       </c>
       <c r="P235" s="2">
         <f>RATE(50,,J185,-'Real Returns 1792-2025'!$J235)</f>
-        <v>8.0393109582212768E-2</v>
+        <v>8.027231653985574E-2</v>
       </c>
       <c r="Q235" s="2">
         <f>RATE(50,,K185,-'Real Returns 1792-2025'!$K235)</f>
-        <v>3.8341820098393153E-2</v>
+        <v>3.8225728588419883E-2</v>
       </c>
       <c r="R235" s="2">
         <f>RATE(100,,J135,-'Real Returns 1792-2025'!$J235)</f>
-        <v>7.0435218073279598E-2</v>
+        <v>7.0375376549018182E-2</v>
       </c>
       <c r="S235" s="2">
         <f>RATE(100,,K135,-'Real Returns 1792-2025'!$K235)</f>
-        <v>2.3619282266133905E-2</v>
+        <v>2.3562057936181387E-2</v>
       </c>
     </row>
     <row r="236" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26108,8 +26101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26559,27 +26552,27 @@
       <c r="A12">
         <v>2025</v>
       </c>
-      <c r="D12" s="42">
-        <v>315.89999999999998</v>
+      <c r="D12" s="47">
+        <v>317.67099999999999</v>
       </c>
       <c r="E12" s="12">
         <f t="shared" ref="E12" si="8">1+(D12-D11)/D11</f>
-        <v>1.0242626054983999</v>
+        <v>1.0300048311215011</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" ref="F12" si="9">E12-1</f>
-        <v>2.426260549839987E-2</v>
+        <v>3.0004831121501097E-2</v>
       </c>
       <c r="G12" s="22">
         <f>VTI!E73-1</f>
         <v>0.26160903455164708</v>
       </c>
       <c r="H12" s="22">
-        <v>0.23172419629412899</v>
+        <v>0.22485739525897963</v>
       </c>
       <c r="I12" s="12">
         <f t="shared" si="1"/>
-        <v>0.23172419629412899</v>
+        <v>0.22485739525897963</v>
       </c>
       <c r="J12" s="30">
         <f>VCLT!E98-1</f>
@@ -26587,15 +26580,15 @@
       </c>
       <c r="K12" s="12">
         <f t="shared" si="2"/>
-        <v>-3.0530981189032635E-2</v>
+        <v>-3.5935722674135917E-2</v>
       </c>
       <c r="L12" s="12">
         <f t="shared" si="3"/>
-        <v>1099727.5825945265</v>
+        <v>1093596.6561052501</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="4"/>
-        <v>8066.952243452889</v>
+        <v>8021.9793865564288</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>